<commit_message>
Added permutations to calculate max ss combinations
</commit_message>
<xml_diff>
--- a/drivers.xlsx
+++ b/drivers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hh\Downloads\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{559C01EF-0030-43CB-9103-DBFB9F1B5A7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACD7EBD-3AA5-4A73-9565-3E49B552B214}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{32EFD6D8-D4DB-4FEE-84AD-AB40F508A809}"/>
+    <workbookView xWindow="60165" yWindow="2745" windowWidth="21600" windowHeight="11385" xr2:uid="{32EFD6D8-D4DB-4FEE-84AD-AB40F508A809}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Aaron </t>
   </si>
@@ -49,39 +49,6 @@
   </si>
   <si>
     <t>Pinto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abelino </t>
-  </si>
-  <si>
-    <t>Solis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adam </t>
-  </si>
-  <si>
-    <t>Gilley</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alex </t>
-  </si>
-  <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <t>Harrison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amy </t>
-  </si>
-  <si>
-    <t>Schares</t>
-  </si>
-  <si>
-    <t>Andy</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kaiser</t>
   </si>
 </sst>
 </file>
@@ -433,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF53E94F-B1BD-404F-B1F0-6ECB5126041B}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A5" sqref="A5:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,54 +444,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>